<commit_message>
imroved document based on review comments
</commit_message>
<xml_diff>
--- a/Template_Files/02_HazardAnalysisAndRiskAssessment_Template.xlsx
+++ b/Template_Files/02_HazardAnalysisAndRiskAssessment_Template.xlsx
@@ -173,7 +173,7 @@
     <t xml:space="preserve">The Lane Departure Warning acting randomly when the camera sensor is not working.</t>
   </si>
   <si>
-    <t xml:space="preserve">city driving is part of regular driving, however </t>
+    <t xml:space="preserve">city driving is part of regular driving</t>
   </si>
   <si>
     <t xml:space="preserve">Collisions at low speed should not cause fatal injuries.</t>
@@ -191,52 +191,52 @@
     <t xml:space="preserve">HA-002</t>
   </si>
   <si>
+    <t xml:space="preserve">Normal Driving on Country Road during Normal conditions with High speed and incorrectly used system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane Keeping Assistance (LKA) function shall apply the steering torque when active in order to stay in ego lane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane Keeping function is always activated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver use the function as if the car was a self-driving car and loose driving attention.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The driver does not use the function properly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country road driving at high speed and together with LKA should not happen often</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collisions at high speed could cause fatal injuries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the driver loose control of the vehicle it is very difficult to realize the situation and act accordingly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Lane Keeping Assistance function shall be time limited, and additional steering torque shall end after a given time interval so the driver cannot misuse the system for autonomous driving.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HA-003</t>
+  </si>
+  <si>
     <t xml:space="preserve">Normal Driving on Country Road during Normal conditions with Low speed</t>
   </si>
   <si>
     <t xml:space="preserve">country driving is part of regular driving</t>
   </si>
   <si>
-    <t xml:space="preserve">HA-003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal Driving on Highway during Normal conditions with High speed and incorrectly used system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane Keeping Assistance (LKA) function shall apply the steering torque when active in order to stay in ego lane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane Keeping function is always activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Driver use the function as if the car was a self-driving car and loose driving attention.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The driver do not use the function properly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">highway driving is part of regular driving and misusing system should not happen often</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collisions at high speed could cause fatal injuries.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When the driver loose control of the vehicle it is very difficult to realize the situation and act accordingly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Lane Keeping Assistance function shall be time limited, and additional steering torque shall end after a given time interval so the driver cannot misuse the system for autonomous driving.</t>
-  </si>
-  <si>
     <t xml:space="preserve">HA-004</t>
   </si>
   <si>
     <t xml:space="preserve">Normal Driving on Mountain Pass during Normal conditions with High speed and incorrectly used system</t>
   </si>
   <si>
-    <t xml:space="preserve">mountain pass driving together with misusing system should not happen often</t>
+    <t xml:space="preserve">mountain pass driving at high speed together with misusing system should not happen often</t>
   </si>
   <si>
     <t xml:space="preserve">EXAMPLE DISCUSSED IN THE PROJECT INSTRUCTIONS - Headlamp System</t>
@@ -420,9 +420,6 @@
     <t xml:space="preserve">Since there is usually no other form of illumination to be expected on country road, it will be difficult for the average driver to control the vehicle in such a situation</t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
     <t xml:space="preserve">HA-005</t>
   </si>
   <si>
@@ -865,6 +862,9 @@
   </si>
   <si>
     <t xml:space="preserve">Less than 90 % of all drivers or other traffic participants are usually able, or barely able, to avoid harm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -1451,10 +1451,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB15"/>
+  <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1960,7 +1960,7 @@
       <c r="AA12" s="17"/>
       <c r="AB12" s="17"/>
     </row>
-    <row r="13" customFormat="false" ht="79.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="92.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
         <v>43</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>OM03 - Normal driving</v>
       </c>
       <c r="C13" s="13" t="str">
-        <f aca="false">'Situational Analysis Guidewords'!D20</f>
+        <f aca="false">'Situational Analysis Guidewords'!$D20</f>
         <v>OS03 - Country Road</v>
       </c>
       <c r="D13" s="14" t="str">
@@ -1977,152 +1977,152 @@
         <v>EN01 - Normal conditions</v>
       </c>
       <c r="E13" s="13" t="str">
-        <f aca="false">'Situational Analysis Guidewords'!$D$33</f>
-        <v>SD01 - Low speed</v>
+        <f aca="false">'Situational Analysis Guidewords'!$D$34</f>
+        <v>SD02 - High speed</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="str">
-        <f aca="false">'Situational Analysis Guidewords'!$D$44</f>
-        <v>IU01 - Correctly used</v>
+        <f aca="false">'Situational Analysis Guidewords'!$D$45</f>
+        <v>IU02 - Incorrectly used</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>44</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="J13" s="13" t="str">
         <f aca="false">'Hazard Analysis Guidewords'!$D$6</f>
         <v>DV03 - Function always activated</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="L13" s="13" t="str">
         <f aca="false">'Hazard Analysis Guidewords'!$D$35</f>
         <v>EV00 - Collision with other vehicle</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>37</v>
+        <v>47</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="O13" s="13" t="str">
-        <f aca="false">'Severity, Exposure, Controllabi'!$E$6</f>
-        <v>E3 - Medium probability</v>
+        <f aca="false">'Severity, Exposure, Controllabi'!$E$5</f>
+        <v>E2 - Low probability</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="Q13" s="13" t="str">
-        <f aca="false">'Severity, Exposure, Controllabi'!$E$13</f>
-        <v>S1 - Light and moderate injuries</v>
+        <f aca="false">'Severity, Exposure, Controllabi'!$E$15</f>
+        <v>S3 - Life-threatening or fatal injuries</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="S13" s="13" t="str">
         <f aca="false">'Severity, Exposure, Controllabi'!$E$23</f>
         <v>C3 - Difficult to control or uncontrollable</v>
       </c>
       <c r="T13" s="13" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="U13" s="13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="V13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="17"/>
-      <c r="AA13" s="17"/>
-      <c r="AB13" s="17"/>
-    </row>
-    <row r="14" customFormat="false" ht="92.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+    </row>
+    <row r="14" customFormat="false" ht="79.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B14" s="13" t="str">
         <f aca="false">'Situational Analysis Guidewords'!$D$7</f>
         <v>OM03 - Normal driving</v>
       </c>
       <c r="C14" s="13" t="str">
-        <f aca="false">'Situational Analysis Guidewords'!$D21</f>
-        <v>OS04 - Highway</v>
+        <f aca="false">'Situational Analysis Guidewords'!D20</f>
+        <v>OS03 - Country Road</v>
       </c>
       <c r="D14" s="14" t="str">
         <f aca="false">'Situational Analysis Guidewords'!$D$51</f>
         <v>EN01 - Normal conditions</v>
       </c>
       <c r="E14" s="13" t="str">
-        <f aca="false">'Situational Analysis Guidewords'!$D$34</f>
-        <v>SD02 - High speed</v>
+        <f aca="false">'Situational Analysis Guidewords'!$D$33</f>
+        <v>SD01 - Low speed</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="str">
-        <f aca="false">'Situational Analysis Guidewords'!$D$45</f>
-        <v>IU02 - Incorrectly used</v>
+        <f aca="false">'Situational Analysis Guidewords'!$D$44</f>
+        <v>IU01 - Correctly used</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="J14" s="13" t="str">
         <f aca="false">'Hazard Analysis Guidewords'!$D$6</f>
         <v>DV03 - Function always activated</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="L14" s="13" t="str">
         <f aca="false">'Hazard Analysis Guidewords'!$D$35</f>
         <v>EV00 - Collision with other vehicle</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="N14" s="13" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="O14" s="13" t="str">
         <f aca="false">'Severity, Exposure, Controllabi'!$E$6</f>
         <v>E3 - Medium probability</v>
       </c>
       <c r="P14" s="13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q14" s="13" t="str">
-        <f aca="false">'Severity, Exposure, Controllabi'!$E$15</f>
-        <v>S3 - Life-threatening or fatal injuries</v>
+        <f aca="false">'Severity, Exposure, Controllabi'!$E$13</f>
+        <v>S1 - Light and moderate injuries</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="S14" s="13" t="str">
         <f aca="false">'Severity, Exposure, Controllabi'!$E$23</f>
         <v>C3 - Difficult to control or uncontrollable</v>
       </c>
       <c r="T14" s="13" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="U14" s="13" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="V14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="19"/>
-      <c r="AA14" s="19"/>
-      <c r="AB14" s="19"/>
+        <v>42</v>
+      </c>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="102.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
@@ -2153,24 +2153,24 @@
         <v>58</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J15" s="13" t="str">
         <f aca="false">'Hazard Analysis Guidewords'!$D$6</f>
         <v>DV03 - Function always activated</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L15" s="13" t="str">
         <f aca="false">'Hazard Analysis Guidewords'!$D$35</f>
         <v>EV00 - Collision with other vehicle</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O15" s="13" t="str">
         <f aca="false">'Severity, Exposure, Controllabi'!$E$4</f>
@@ -2184,20 +2184,20 @@
         <v>S3 - Life-threatening or fatal injuries</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="S15" s="13" t="str">
         <f aca="false">'Severity, Exposure, Controllabi'!$E$23</f>
         <v>C3 - Difficult to control or uncontrollable</v>
       </c>
       <c r="T15" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U15" s="13" t="s">
         <v>41</v>
       </c>
       <c r="V15" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="W15" s="18"/>
       <c r="X15" s="18"/>
@@ -2206,6 +2206,7 @@
       <c r="AA15" s="19"/>
       <c r="AB15" s="19"/>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B10:H10"/>
@@ -2956,7 +2957,7 @@
     </row>
     <row r="16" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="28" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>85</v>
@@ -3075,7 +3076,7 @@
         <v>75</v>
       </c>
       <c r="Q17" s="28" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="R17" s="28" t="s">
         <v>108</v>
@@ -3090,7 +3091,7 @@
         <v>119</v>
       </c>
       <c r="V17" s="28" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="W17" s="29" t="s">
         <v>93</v>
@@ -3104,7 +3105,7 @@
     </row>
     <row r="18" customFormat="false" ht="60.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>85</v>
@@ -3116,7 +3117,7 @@
         <v>94</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="28" t="s">
         <v>95</v>
@@ -3125,7 +3126,7 @@
         <v>89</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J18" s="28" t="s">
         <v>69</v>
@@ -3149,7 +3150,7 @@
         <v>106</v>
       </c>
       <c r="Q18" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R18" s="28" t="s">
         <v>108</v>
@@ -3158,13 +3159,13 @@
         <v>118</v>
       </c>
       <c r="T18" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U18" s="28" t="s">
         <v>119</v>
       </c>
       <c r="V18" s="28" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="W18" s="29" t="s">
         <v>93</v>
@@ -4118,7 +4119,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -4205,16 +4206,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="C4" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="D4" s="32" t="s">
         <v>129</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>130</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
@@ -4245,10 +4246,10 @@
         <v>OM01</v>
       </c>
       <c r="B5" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>131</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>132</v>
       </c>
       <c r="D5" s="35" t="str">
         <f aca="false">$A5 &amp; " - " &amp; $B5</f>
@@ -4283,10 +4284,10 @@
         <v>OM02</v>
       </c>
       <c r="B6" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="34" t="s">
         <v>133</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>134</v>
       </c>
       <c r="D6" s="35" t="str">
         <f aca="false">$A6 &amp; " - " &amp; $B6</f>
@@ -4321,10 +4322,10 @@
         <v>OM03</v>
       </c>
       <c r="B7" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>135</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>136</v>
       </c>
       <c r="D7" s="35" t="str">
         <f aca="false">$A7 &amp; " - " &amp; $B7</f>
@@ -4359,10 +4360,10 @@
         <v>OM04</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D8" s="35" t="str">
         <f aca="false">$A8 &amp; " - " &amp; $B8</f>
@@ -4397,10 +4398,10 @@
         <v>OM05</v>
       </c>
       <c r="B9" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>138</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>139</v>
       </c>
       <c r="D9" s="35" t="str">
         <f aca="false">$A9 &amp; " - " &amp; $B9</f>
@@ -4435,10 +4436,10 @@
         <v>OM06</v>
       </c>
       <c r="B10" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="34" t="s">
         <v>140</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>141</v>
       </c>
       <c r="D10" s="35" t="str">
         <f aca="false">$A10 &amp; " - " &amp; $B10</f>
@@ -4473,10 +4474,10 @@
         <v>OM07</v>
       </c>
       <c r="B11" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>142</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>143</v>
       </c>
       <c r="D11" s="35" t="str">
         <f aca="false">$A11 &amp; " - " &amp; $B11</f>
@@ -4511,10 +4512,10 @@
         <v>OM08</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>144</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>145</v>
       </c>
       <c r="D12" s="35" t="str">
         <f aca="false">$A12 &amp; " - " &amp; $B12</f>
@@ -4549,10 +4550,10 @@
         <v>OM09</v>
       </c>
       <c r="B13" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="D13" s="35" t="str">
         <f aca="false">$A13 &amp; " - " &amp; $B13</f>
@@ -4669,16 +4670,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C17" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="32" t="s">
         <v>129</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>130</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
@@ -4709,10 +4710,10 @@
         <v>OS01</v>
       </c>
       <c r="B18" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="34" t="s">
         <v>149</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>150</v>
       </c>
       <c r="D18" s="35" t="str">
         <f aca="false">$A18 &amp; " - " &amp; $B18</f>
@@ -4750,7 +4751,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" s="35" t="str">
         <f aca="false">$A19 &amp; " - " &amp; $B19</f>
@@ -4785,10 +4786,10 @@
         <v>OS03</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D20" s="35" t="str">
         <f aca="false">$A20 &amp; " - " &amp; $B20</f>
@@ -4823,10 +4824,10 @@
         <v>OS04</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" s="35" t="str">
         <f aca="false">$A21 &amp; " - " &amp; $B21</f>
@@ -4861,10 +4862,10 @@
         <v>OS05</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D22" s="35" t="str">
         <f aca="false">$A22 &amp; " - " &amp; $B22</f>
@@ -4899,10 +4900,10 @@
         <v>OS06</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D23" s="35" t="str">
         <f aca="false">$A23 &amp; " - " &amp; $B23</f>
@@ -4937,10 +4938,10 @@
         <v>OS07</v>
       </c>
       <c r="B24" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="34" t="s">
         <v>155</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>156</v>
       </c>
       <c r="D24" s="35" t="str">
         <f aca="false">$A24 &amp; " - " &amp; $B24</f>
@@ -4975,10 +4976,10 @@
         <v>OS08</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D25" s="35" t="str">
         <f aca="false">$A25 &amp; " - " &amp; $B25</f>
@@ -5013,10 +5014,10 @@
         <v>OS09</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" s="35" t="str">
         <f aca="false">$A26 &amp; " - " &amp; $B26</f>
@@ -5051,10 +5052,10 @@
         <v>OS10</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D27" s="35" t="str">
         <f aca="false">$A27 &amp; " - " &amp; $B27</f>
@@ -5089,10 +5090,10 @@
         <v>OS11</v>
       </c>
       <c r="B28" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="D28" s="35" t="str">
         <f aca="false">$A28 &amp; " - " &amp; $B28</f>
@@ -5209,16 +5210,16 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="32" t="s">
         <v>129</v>
-      </c>
-      <c r="D32" s="32" t="s">
-        <v>130</v>
       </c>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
@@ -5249,10 +5250,10 @@
         <v>SD01</v>
       </c>
       <c r="B33" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="34" t="s">
         <v>160</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>161</v>
       </c>
       <c r="D33" s="35" t="str">
         <f aca="false">$A33 &amp; " - " &amp; $B33</f>
@@ -5287,10 +5288,10 @@
         <v>SD02</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D34" s="35" t="str">
         <f aca="false">$A34 &amp; " - " &amp; $B34</f>
@@ -5325,10 +5326,10 @@
         <v>SD03</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D35" s="35" t="str">
         <f aca="false">$A35 &amp; " - " &amp; $B35</f>
@@ -5363,10 +5364,10 @@
         <v>SD04</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D36" s="35" t="str">
         <f aca="false">$A36 &amp; " - " &amp; $B36</f>
@@ -5401,10 +5402,10 @@
         <v>SD05</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D37" s="35" t="str">
         <f aca="false">$A37 &amp; " - " &amp; $B37</f>
@@ -5439,10 +5440,10 @@
         <v>SD06</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D38" s="35" t="str">
         <f aca="false">$A38 &amp; " - " &amp; $B38</f>
@@ -5477,10 +5478,10 @@
         <v>SD07</v>
       </c>
       <c r="B39" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="D39" s="35" t="str">
         <f aca="false">$A39 &amp; " - " &amp; $B39</f>
@@ -5567,7 +5568,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -5597,16 +5598,16 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="C43" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="D43" s="32" t="s">
         <v>129</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>130</v>
       </c>
       <c r="E43" s="21"/>
       <c r="F43" s="21"/>
@@ -5637,10 +5638,10 @@
         <v>IU01</v>
       </c>
       <c r="B44" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" s="34" t="s">
         <v>168</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>169</v>
       </c>
       <c r="D44" s="35" t="str">
         <f aca="false">$A44 &amp; " - " &amp; $B44</f>
@@ -5675,10 +5676,10 @@
         <v>IU02</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C45" s="34" t="s">
         <v>170</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>171</v>
       </c>
       <c r="D45" s="35" t="str">
         <f aca="false">$A45 &amp; " - " &amp; $B45</f>
@@ -5713,10 +5714,10 @@
         <v>IU03</v>
       </c>
       <c r="B46" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="D46" s="35" t="str">
         <f aca="false">$A46 &amp; " - " &amp; $B46</f>
@@ -5833,16 +5834,16 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C50" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="32" t="s">
         <v>129</v>
-      </c>
-      <c r="D50" s="32" t="s">
-        <v>130</v>
       </c>
       <c r="E50" s="21"/>
       <c r="F50" s="21"/>
@@ -5873,10 +5874,10 @@
         <v>EN01</v>
       </c>
       <c r="B51" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C51" s="34" t="s">
         <v>172</v>
-      </c>
-      <c r="C51" s="34" t="s">
-        <v>173</v>
       </c>
       <c r="D51" s="35" t="str">
         <f aca="false">$A51 &amp; " - " &amp; $B51</f>
@@ -5911,10 +5912,10 @@
         <v>EN02</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D52" s="35" t="str">
         <f aca="false">$A52 &amp; " - " &amp; $B52</f>
@@ -5949,10 +5950,10 @@
         <v>EN03</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D53" s="35" t="str">
         <f aca="false">$A53 &amp; " - " &amp; $B53</f>
@@ -5987,10 +5988,10 @@
         <v>EN04</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C54" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D54" s="35" t="str">
         <f aca="false">$A54 &amp; " - " &amp; $B54</f>
@@ -6025,10 +6026,10 @@
         <v>EN05</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C55" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D55" s="35" t="str">
         <f aca="false">$A55 &amp; " - " &amp; $B55</f>
@@ -6063,10 +6064,10 @@
         <v>EN06</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C56" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D56" s="35" t="str">
         <f aca="false">$A56 &amp; " - " &amp; $B56</f>
@@ -6101,10 +6102,10 @@
         <v>EN07</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C57" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D57" s="35" t="str">
         <f aca="false">$A57 &amp; " - " &amp; $B57</f>
@@ -6139,10 +6140,10 @@
         <v>EN08</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D58" s="35" t="str">
         <f aca="false">$A58 &amp; " - " &amp; $B58</f>
@@ -6177,10 +6178,10 @@
         <v>EN09</v>
       </c>
       <c r="B59" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="C59" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="D59" s="35" t="str">
         <f aca="false">$A59 &amp; " - " &amp; $B59</f>
@@ -7232,16 +7233,16 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C3" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>129</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>130</v>
       </c>
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
@@ -7275,7 +7276,7 @@
         <v>70</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D4" s="35" t="str">
         <f aca="false">$A4 &amp; " - " &amp; $B4</f>
@@ -7310,10 +7311,10 @@
         <v>DV02</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5" s="35" t="str">
         <f aca="false">$A5 &amp; " - " &amp; $B5</f>
@@ -7348,10 +7349,10 @@
         <v>DV03</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D6" s="35" t="str">
         <f aca="false">$A6 &amp; " - " &amp; $B6</f>
@@ -7386,10 +7387,10 @@
         <v>DV04</v>
       </c>
       <c r="B7" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>185</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>186</v>
       </c>
       <c r="D7" s="35" t="str">
         <f aca="false">$A7 &amp; " - " &amp; $B7</f>
@@ -7424,10 +7425,10 @@
         <v>DV05</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8" s="35" t="str">
         <f aca="false">$A8 &amp; " - " &amp; $B8</f>
@@ -7462,10 +7463,10 @@
         <v>DV06</v>
       </c>
       <c r="B9" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>188</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>189</v>
       </c>
       <c r="D9" s="35" t="str">
         <f aca="false">$A9 &amp; " - " &amp; $B9</f>
@@ -7500,10 +7501,10 @@
         <v>DV07</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D10" s="35" t="str">
         <f aca="false">$A10 &amp; " - " &amp; $B10</f>
@@ -7538,10 +7539,10 @@
         <v>DV08</v>
       </c>
       <c r="B11" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>191</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>192</v>
       </c>
       <c r="D11" s="35" t="str">
         <f aca="false">$A11 &amp; " - " &amp; $B11</f>
@@ -7576,10 +7577,10 @@
         <v>DV09</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D12" s="35" t="str">
         <f aca="false">$A12 &amp; " - " &amp; $B12</f>
@@ -7614,10 +7615,10 @@
         <v>DV10</v>
       </c>
       <c r="B13" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="34" t="s">
         <v>194</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>195</v>
       </c>
       <c r="D13" s="35" t="str">
         <f aca="false">$A13 &amp; " - " &amp; $B13</f>
@@ -7652,10 +7653,10 @@
         <v>DV11</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D14" s="35" t="str">
         <f aca="false">$A14 &amp; " - " &amp; $B14</f>
@@ -7690,10 +7691,10 @@
         <v>DV12</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" s="35" t="str">
         <f aca="false">$A15 &amp; " - " &amp; $B15</f>
@@ -7728,10 +7729,10 @@
         <v>DV13</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D16" s="35" t="str">
         <f aca="false">$A16 &amp; " - " &amp; $B16</f>
@@ -7766,10 +7767,10 @@
         <v>DV14</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" s="35" t="str">
         <f aca="false">$A17 &amp; " - " &amp; $B17</f>
@@ -7804,10 +7805,10 @@
         <v>DV15</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" s="35" t="str">
         <f aca="false">$A18 &amp; " - " &amp; $B18</f>
@@ -7842,10 +7843,10 @@
         <v>DV16</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D19" s="35" t="str">
         <f aca="false">$A19 &amp; " - " &amp; $B19</f>
@@ -7880,10 +7881,10 @@
         <v>DV17</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D20" s="35" t="str">
         <f aca="false">$A20 &amp; " - " &amp; $B20</f>
@@ -7918,10 +7919,10 @@
         <v>DV18</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D21" s="35" t="str">
         <f aca="false">$A21 &amp; " - " &amp; $B21</f>
@@ -7956,10 +7957,10 @@
         <v>DV19</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D22" s="35" t="str">
         <f aca="false">$A22 &amp; " - " &amp; $B22</f>
@@ -7994,10 +7995,10 @@
         <v>DV20</v>
       </c>
       <c r="B23" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="D23" s="35" t="str">
         <f aca="false">$A23 &amp; " - " &amp; $B23</f>
@@ -8084,7 +8085,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
@@ -8114,16 +8115,16 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C27" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="43" t="s">
         <v>129</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>130</v>
       </c>
       <c r="E27" s="38"/>
       <c r="F27" s="38"/>
@@ -8154,7 +8155,7 @@
         <v>EV-07</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C28" s="46"/>
       <c r="D28" s="47" t="str">
@@ -8190,7 +8191,7 @@
         <v>EV-06</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C29" s="46"/>
       <c r="D29" s="47" t="str">
@@ -8226,7 +8227,7 @@
         <v>EV-05</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C30" s="46"/>
       <c r="D30" s="47" t="str">
@@ -8298,7 +8299,7 @@
         <v>EV-03</v>
       </c>
       <c r="B32" s="45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C32" s="46"/>
       <c r="D32" s="47" t="str">
@@ -8334,7 +8335,7 @@
         <v>EV-02</v>
       </c>
       <c r="B33" s="45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C33" s="46"/>
       <c r="D33" s="47" t="str">
@@ -8370,7 +8371,7 @@
         <v>EV-01</v>
       </c>
       <c r="B34" s="45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C34" s="46"/>
       <c r="D34" s="47" t="str">
@@ -8406,7 +8407,7 @@
         <v>EV00</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C35" s="46"/>
       <c r="D35" s="47" t="str">
@@ -8442,7 +8443,7 @@
         <v>EV01</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C36" s="46"/>
       <c r="D36" s="47" t="str">
@@ -8478,7 +8479,7 @@
         <v>EV02</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C37" s="46"/>
       <c r="D37" s="47" t="str">
@@ -8514,7 +8515,7 @@
         <v>EV03</v>
       </c>
       <c r="B38" s="45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C38" s="46"/>
       <c r="D38" s="47" t="str">
@@ -8550,7 +8551,7 @@
         <v>EV04</v>
       </c>
       <c r="B39" s="45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C39" s="46"/>
       <c r="D39" s="47" t="str">
@@ -8586,7 +8587,7 @@
         <v>EV05</v>
       </c>
       <c r="B40" s="45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C40" s="46"/>
       <c r="D40" s="47" t="str">
@@ -8622,7 +8623,7 @@
         <v>EV06</v>
       </c>
       <c r="B41" s="45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C41" s="46"/>
       <c r="D41" s="47" t="str">
@@ -8714,7 +8715,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -8744,19 +8745,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="D2" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>222</v>
-      </c>
       <c r="E2" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
@@ -8782,10 +8783,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="34" t="s">
         <v>223</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>224</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -8817,16 +8818,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="C4" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="D4" s="34" t="s">
         <v>227</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>228</v>
       </c>
       <c r="E4" s="35" t="str">
         <f aca="false">$A4 &amp; " - " &amp; $B4</f>
@@ -8856,16 +8857,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="C5" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="D5" s="34" t="s">
         <v>231</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>232</v>
       </c>
       <c r="E5" s="35" t="str">
         <f aca="false">$A5 &amp; " - " &amp; $B5</f>
@@ -8895,16 +8896,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="C6" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="D6" s="34" t="s">
         <v>235</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>236</v>
       </c>
       <c r="E6" s="35" t="str">
         <f aca="false">$A6 &amp; " - " &amp; $B6</f>
@@ -8934,16 +8935,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="50" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="C7" s="34" t="s">
         <v>238</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="D7" s="34" t="s">
         <v>239</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>240</v>
       </c>
       <c r="E7" s="35" t="str">
         <f aca="false">$A7 &amp; " - " &amp; $B7</f>
@@ -9029,7 +9030,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -9059,19 +9060,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C11" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="E11" s="32" t="s">
         <v>129</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>130</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -9097,16 +9098,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="C12" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>244</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>245</v>
       </c>
       <c r="E12" s="35" t="str">
         <f aca="false">$A12 &amp; " - " &amp; $B12</f>
@@ -9136,16 +9137,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="C13" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>247</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>247</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>248</v>
       </c>
       <c r="E13" s="35" t="str">
         <f aca="false">$A13 &amp; " - " &amp; $B13</f>
@@ -9175,16 +9176,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="C14" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="D14" s="34" t="s">
         <v>251</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>252</v>
       </c>
       <c r="E14" s="35" t="str">
         <f aca="false">$A14 &amp; " - " &amp; $B14</f>
@@ -9214,16 +9215,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="50" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="C15" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="D15" s="34" t="s">
         <v>255</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>256</v>
       </c>
       <c r="E15" s="35" t="str">
         <f aca="false">$A15 &amp; " - " &amp; $B15</f>
@@ -9309,7 +9310,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -9339,17 +9340,17 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D19" s="52"/>
       <c r="E19" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
@@ -9375,13 +9376,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="B20" s="34" t="s">
-        <v>259</v>
-      </c>
       <c r="C20" s="53" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D20" s="54"/>
       <c r="E20" s="35" t="str">
@@ -9412,13 +9413,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="B21" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="C21" s="53" t="s">
         <v>261</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>262</v>
       </c>
       <c r="D21" s="54"/>
       <c r="E21" s="35" t="str">
@@ -9449,13 +9450,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>263</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="C22" s="53" t="s">
         <v>264</v>
-      </c>
-      <c r="C22" s="53" t="s">
-        <v>265</v>
       </c>
       <c r="D22" s="54"/>
       <c r="E22" s="35" t="str">
@@ -9486,13 +9487,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="C23" s="53" t="s">
         <v>267</v>
-      </c>
-      <c r="C23" s="53" t="s">
-        <v>268</v>
       </c>
       <c r="D23" s="54"/>
       <c r="E23" s="35" t="str">
@@ -9568,7 +9569,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9578,13 +9579,13 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E2" s="59"/>
       <c r="F2" s="59"/>
@@ -9594,24 +9595,24 @@
       <c r="B3" s="57"/>
       <c r="C3" s="58"/>
       <c r="D3" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="60" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D4" s="61" t="s">
         <v>81</v>
@@ -9629,7 +9630,7 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="60"/>
       <c r="C5" s="61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D5" s="61" t="s">
         <v>81</v>
@@ -9647,7 +9648,7 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="60"/>
       <c r="C6" s="61" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="61" t="s">
         <v>81</v>
@@ -9665,7 +9666,7 @@
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="60"/>
       <c r="C7" s="61" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D7" s="61" t="s">
         <v>81</v>
@@ -9677,15 +9678,15 @@
         <v>41</v>
       </c>
       <c r="G7" s="61" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="60" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D8" s="61" t="s">
         <v>81</v>
@@ -9703,7 +9704,7 @@
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="60"/>
       <c r="C9" s="61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D9" s="61" t="s">
         <v>81</v>
@@ -9721,7 +9722,7 @@
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="60"/>
       <c r="C10" s="61" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D10" s="61" t="s">
         <v>81</v>
@@ -9733,13 +9734,13 @@
         <v>41</v>
       </c>
       <c r="G10" s="61" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="60"/>
       <c r="C11" s="61" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D11" s="61" t="s">
         <v>81</v>
@@ -9748,18 +9749,18 @@
         <v>41</v>
       </c>
       <c r="F11" s="61" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>55</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D12" s="61" t="s">
         <v>81</v>
@@ -9777,7 +9778,7 @@
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="60"/>
       <c r="C13" s="61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D13" s="61" t="s">
         <v>81</v>
@@ -9789,13 +9790,13 @@
         <v>41</v>
       </c>
       <c r="G13" s="61" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="60"/>
       <c r="C14" s="61" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D14" s="61" t="s">
         <v>81</v>
@@ -9804,25 +9805,25 @@
         <v>41</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="G14" s="61" t="s">
-        <v>55</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="60"/>
       <c r="C15" s="61" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D15" s="61" t="s">
         <v>81</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="F15" s="61" t="s">
-        <v>55</v>
+        <v>268</v>
       </c>
       <c r="G15" s="61" t="s">
         <v>269</v>

</xml_diff>